<commit_message>
filtered Km calculation for exponential growth phase only
</commit_message>
<xml_diff>
--- a/data/2018_Silverman_et_al-heterocyst_data_summary.xlsx
+++ b/data/2018_Silverman_et_al-heterocyst_data_summary.xlsx
@@ -425,13 +425,13 @@
         <v>9.33437013996889</v>
       </c>
       <c r="F2" t="n">
-        <v>0.172253206300272</v>
+        <v>0.172905782177114</v>
       </c>
       <c r="G2" t="n">
         <v>9</v>
       </c>
       <c r="H2" t="n">
-        <v>0.476721368582596</v>
+        <v>0.479568541489103</v>
       </c>
     </row>
     <row r="3">
@@ -451,13 +451,13 @@
         <v>9.41575492341357</v>
       </c>
       <c r="F3" t="n">
-        <v>0.199665905482454</v>
+        <v>0.200262315313081</v>
       </c>
       <c r="G3" t="n">
         <v>9</v>
       </c>
       <c r="H3" t="n">
-        <v>0.469101328132906</v>
+        <v>0.457945099017026</v>
       </c>
     </row>
     <row r="4">
@@ -477,13 +477,13 @@
         <v>11.5638051044084</v>
       </c>
       <c r="F4" t="n">
-        <v>0.248757258059664</v>
+        <v>0.25022116058967</v>
       </c>
       <c r="G4" t="n">
         <v>12</v>
       </c>
       <c r="H4" t="n">
-        <v>0.534978693222639</v>
+        <v>0.540270202668898</v>
       </c>
     </row>
     <row r="5">
@@ -503,13 +503,13 @@
         <v>12.8737060041408</v>
       </c>
       <c r="F5" t="n">
-        <v>0.267529967255851</v>
+        <v>0.268341012420777</v>
       </c>
       <c r="G5" t="n">
         <v>12</v>
       </c>
       <c r="H5" t="n">
-        <v>0.498766245617892</v>
+        <v>0.498401850322011</v>
       </c>
     </row>
     <row r="6">
@@ -529,13 +529,13 @@
         <v>7.69918699186992</v>
       </c>
       <c r="F6" t="n">
-        <v>0.309351349624615</v>
+        <v>0.308198658675583</v>
       </c>
       <c r="G6" t="n">
         <v>7</v>
       </c>
       <c r="H6" t="n">
-        <v>0.49858257549235</v>
+        <v>0.490220681240925</v>
       </c>
     </row>
     <row r="7">
@@ -555,13 +555,13 @@
         <v>11.0650887573964</v>
       </c>
       <c r="F7" t="n">
-        <v>0.28790591185566</v>
+        <v>0.290216547300712</v>
       </c>
       <c r="G7" t="n">
         <v>11</v>
       </c>
       <c r="H7" t="n">
-        <v>0.399894881082411</v>
+        <v>0.399285836436981</v>
       </c>
     </row>
     <row r="8">
@@ -581,13 +581,13 @@
         <v>12.6979865771812</v>
       </c>
       <c r="F8" t="n">
-        <v>0.287700673587536</v>
+        <v>0.289015053142963</v>
       </c>
       <c r="G8" t="n">
         <v>12</v>
       </c>
       <c r="H8" t="n">
-        <v>0.4867922726551</v>
+        <v>0.49241595574623</v>
       </c>
     </row>
     <row r="9">
@@ -607,13 +607,13 @@
         <v>13.8702702702703</v>
       </c>
       <c r="F9" t="n">
-        <v>0.280875507150911</v>
+        <v>0.278280443974346</v>
       </c>
       <c r="G9" t="n">
         <v>14</v>
       </c>
       <c r="H9" t="n">
-        <v>0.473934979047089</v>
+        <v>0.470235176397004</v>
       </c>
     </row>
     <row r="10">
@@ -633,13 +633,13 @@
         <v>16.272</v>
       </c>
       <c r="F10" t="n">
-        <v>0.475375923256966</v>
+        <v>0.473212165263482</v>
       </c>
       <c r="G10" t="n">
         <v>15</v>
       </c>
       <c r="H10" t="n">
-        <v>0.544632329534682</v>
+        <v>0.551546193172615</v>
       </c>
     </row>
     <row r="11">
@@ -659,13 +659,13 @@
         <v>8.0995145631068</v>
       </c>
       <c r="F11" t="n">
-        <v>0.182751306265823</v>
+        <v>0.182520216912646</v>
       </c>
       <c r="G11" t="n">
         <v>8</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0611022379580608</v>
+        <v>0.0499348925451281</v>
       </c>
     </row>
     <row r="12">
@@ -685,13 +685,13 @@
         <v>10.6167979002625</v>
       </c>
       <c r="F12" t="n">
-        <v>0.186327429501234</v>
+        <v>0.186189592176234</v>
       </c>
       <c r="G12" t="n">
         <v>10</v>
       </c>
       <c r="H12" t="n">
-        <v>0.476113888092371</v>
+        <v>0.475337454547499</v>
       </c>
     </row>
     <row r="13">
@@ -711,13 +711,13 @@
         <v>14.8488063660477</v>
       </c>
       <c r="F13" t="n">
-        <v>0.292241694552718</v>
+        <v>0.293061786999847</v>
       </c>
       <c r="G13" t="n">
         <v>14</v>
       </c>
       <c r="H13" t="n">
-        <v>0.447991848917697</v>
+        <v>0.45567932106213</v>
       </c>
     </row>
     <row r="14">
@@ -737,13 +737,13 @@
         <v>16.936</v>
       </c>
       <c r="F14" t="n">
-        <v>0.41872055168621</v>
+        <v>0.417910060029995</v>
       </c>
       <c r="G14" t="n">
         <v>16</v>
       </c>
       <c r="H14" t="n">
-        <v>0.438645825422014</v>
+        <v>0.443094044568794</v>
       </c>
     </row>
     <row r="15">
@@ -763,13 +763,13 @@
         <v>19.1713395638629</v>
       </c>
       <c r="F15" t="n">
-        <v>0.449126226176202</v>
+        <v>0.44673037387372</v>
       </c>
       <c r="G15" t="n">
         <v>18</v>
       </c>
       <c r="H15" t="n">
-        <v>0.724030538182072</v>
+        <v>0.721054033286632</v>
       </c>
     </row>
     <row r="16">
@@ -789,13 +789,13 @@
         <v>20.5544554455446</v>
       </c>
       <c r="F16" t="n">
-        <v>1.11476960150764</v>
+        <v>1.107847845845</v>
       </c>
       <c r="G16" t="n">
         <v>21</v>
       </c>
       <c r="H16" t="n">
-        <v>1.34602629498342</v>
+        <v>1.35901652893772</v>
       </c>
     </row>
     <row r="17">
@@ -815,13 +815,13 @@
         <v>27.40625</v>
       </c>
       <c r="F17" t="n">
-        <v>2.24031699427435</v>
+        <v>2.24732400026869</v>
       </c>
       <c r="G17" t="n">
         <v>25</v>
       </c>
       <c r="H17" t="n">
-        <v>3.08725803297395</v>
+        <v>3.11507539149451</v>
       </c>
     </row>
     <row r="18">
@@ -841,13 +841,13 @@
         <v>27.0641025641026</v>
       </c>
       <c r="F18" t="n">
-        <v>1.70037246091027</v>
+        <v>1.7015621600056</v>
       </c>
       <c r="G18" t="n">
         <v>26</v>
       </c>
       <c r="H18" t="n">
-        <v>1.4235949643851</v>
+        <v>1.42348210431368</v>
       </c>
     </row>
     <row r="19">
@@ -867,13 +867,13 @@
         <v>23.719512195122</v>
       </c>
       <c r="F19" t="n">
-        <v>1.60199758409185</v>
+        <v>1.61298663182518</v>
       </c>
       <c r="G19" t="n">
         <v>23.5</v>
       </c>
       <c r="H19" t="n">
-        <v>2.03003079410757</v>
+        <v>2.01718716138192</v>
       </c>
     </row>
     <row r="20">
@@ -893,13 +893,13 @@
         <v>26.5978260869565</v>
       </c>
       <c r="F20" t="n">
-        <v>1.47293442595309</v>
+        <v>1.49476448346593</v>
       </c>
       <c r="G20" t="n">
         <v>26.5</v>
       </c>
       <c r="H20" t="n">
-        <v>1.76977855002148</v>
+        <v>1.75850222635062</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
re-knit everything for final revisions
</commit_message>
<xml_diff>
--- a/data/2018_Silverman_et_al-heterocyst_data_summary.xlsx
+++ b/data/2018_Silverman_et_al-heterocyst_data_summary.xlsx
@@ -425,13 +425,13 @@
         <v>9.33437013996889</v>
       </c>
       <c r="F2" t="n">
-        <v>0.172905782177114</v>
+        <v>0.172253206300272</v>
       </c>
       <c r="G2" t="n">
         <v>9</v>
       </c>
       <c r="H2" t="n">
-        <v>0.479568541489103</v>
+        <v>0.476721368582596</v>
       </c>
     </row>
     <row r="3">
@@ -451,13 +451,13 @@
         <v>9.41575492341357</v>
       </c>
       <c r="F3" t="n">
-        <v>0.200262315313081</v>
+        <v>0.199665905482454</v>
       </c>
       <c r="G3" t="n">
         <v>9</v>
       </c>
       <c r="H3" t="n">
-        <v>0.457945099017026</v>
+        <v>0.469101328132906</v>
       </c>
     </row>
     <row r="4">
@@ -477,13 +477,13 @@
         <v>11.5638051044084</v>
       </c>
       <c r="F4" t="n">
-        <v>0.25022116058967</v>
+        <v>0.248757258059664</v>
       </c>
       <c r="G4" t="n">
         <v>12</v>
       </c>
       <c r="H4" t="n">
-        <v>0.540270202668898</v>
+        <v>0.534978693222639</v>
       </c>
     </row>
     <row r="5">
@@ -503,13 +503,13 @@
         <v>12.8737060041408</v>
       </c>
       <c r="F5" t="n">
-        <v>0.268341012420777</v>
+        <v>0.267529967255851</v>
       </c>
       <c r="G5" t="n">
         <v>12</v>
       </c>
       <c r="H5" t="n">
-        <v>0.498401850322011</v>
+        <v>0.498766245617892</v>
       </c>
     </row>
     <row r="6">
@@ -529,13 +529,13 @@
         <v>7.69918699186992</v>
       </c>
       <c r="F6" t="n">
-        <v>0.308198658675583</v>
+        <v>0.309351349624615</v>
       </c>
       <c r="G6" t="n">
         <v>7</v>
       </c>
       <c r="H6" t="n">
-        <v>0.490220681240925</v>
+        <v>0.49858257549235</v>
       </c>
     </row>
     <row r="7">
@@ -555,13 +555,13 @@
         <v>11.0650887573964</v>
       </c>
       <c r="F7" t="n">
-        <v>0.290216547300712</v>
+        <v>0.28790591185566</v>
       </c>
       <c r="G7" t="n">
         <v>11</v>
       </c>
       <c r="H7" t="n">
-        <v>0.399285836436981</v>
+        <v>0.399894881082411</v>
       </c>
     </row>
     <row r="8">
@@ -581,13 +581,13 @@
         <v>12.6979865771812</v>
       </c>
       <c r="F8" t="n">
-        <v>0.289015053142963</v>
+        <v>0.287700673587536</v>
       </c>
       <c r="G8" t="n">
         <v>12</v>
       </c>
       <c r="H8" t="n">
-        <v>0.49241595574623</v>
+        <v>0.4867922726551</v>
       </c>
     </row>
     <row r="9">
@@ -607,13 +607,13 @@
         <v>13.8702702702703</v>
       </c>
       <c r="F9" t="n">
-        <v>0.278280443974346</v>
+        <v>0.280875507150911</v>
       </c>
       <c r="G9" t="n">
         <v>14</v>
       </c>
       <c r="H9" t="n">
-        <v>0.470235176397004</v>
+        <v>0.473934979047089</v>
       </c>
     </row>
     <row r="10">
@@ -633,13 +633,13 @@
         <v>16.272</v>
       </c>
       <c r="F10" t="n">
-        <v>0.473212165263482</v>
+        <v>0.475375923256966</v>
       </c>
       <c r="G10" t="n">
         <v>15</v>
       </c>
       <c r="H10" t="n">
-        <v>0.551546193172615</v>
+        <v>0.544632329534682</v>
       </c>
     </row>
     <row r="11">
@@ -659,13 +659,13 @@
         <v>8.0995145631068</v>
       </c>
       <c r="F11" t="n">
-        <v>0.182520216912646</v>
+        <v>0.182751306265823</v>
       </c>
       <c r="G11" t="n">
         <v>8</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0499348925451281</v>
+        <v>0.0611022379580608</v>
       </c>
     </row>
     <row r="12">
@@ -685,13 +685,13 @@
         <v>10.6167979002625</v>
       </c>
       <c r="F12" t="n">
-        <v>0.186189592176234</v>
+        <v>0.186327429501234</v>
       </c>
       <c r="G12" t="n">
         <v>10</v>
       </c>
       <c r="H12" t="n">
-        <v>0.475337454547499</v>
+        <v>0.476113888092371</v>
       </c>
     </row>
     <row r="13">
@@ -711,13 +711,13 @@
         <v>14.8488063660477</v>
       </c>
       <c r="F13" t="n">
-        <v>0.293061786999847</v>
+        <v>0.292241694552718</v>
       </c>
       <c r="G13" t="n">
         <v>14</v>
       </c>
       <c r="H13" t="n">
-        <v>0.45567932106213</v>
+        <v>0.447991848917697</v>
       </c>
     </row>
     <row r="14">
@@ -737,13 +737,13 @@
         <v>16.936</v>
       </c>
       <c r="F14" t="n">
-        <v>0.417910060029995</v>
+        <v>0.41872055168621</v>
       </c>
       <c r="G14" t="n">
         <v>16</v>
       </c>
       <c r="H14" t="n">
-        <v>0.443094044568794</v>
+        <v>0.438645825422014</v>
       </c>
     </row>
     <row r="15">
@@ -763,13 +763,13 @@
         <v>19.1713395638629</v>
       </c>
       <c r="F15" t="n">
-        <v>0.44673037387372</v>
+        <v>0.449126226176202</v>
       </c>
       <c r="G15" t="n">
         <v>18</v>
       </c>
       <c r="H15" t="n">
-        <v>0.721054033286632</v>
+        <v>0.724030538182072</v>
       </c>
     </row>
     <row r="16">
@@ -789,13 +789,13 @@
         <v>20.5544554455446</v>
       </c>
       <c r="F16" t="n">
-        <v>1.107847845845</v>
+        <v>1.11476960150764</v>
       </c>
       <c r="G16" t="n">
         <v>21</v>
       </c>
       <c r="H16" t="n">
-        <v>1.35901652893772</v>
+        <v>1.34602629498342</v>
       </c>
     </row>
     <row r="17">
@@ -815,13 +815,13 @@
         <v>27.40625</v>
       </c>
       <c r="F17" t="n">
-        <v>2.24732400026869</v>
+        <v>2.24031699427435</v>
       </c>
       <c r="G17" t="n">
         <v>25</v>
       </c>
       <c r="H17" t="n">
-        <v>3.11507539149451</v>
+        <v>3.08725803297395</v>
       </c>
     </row>
     <row r="18">
@@ -841,13 +841,13 @@
         <v>27.0641025641026</v>
       </c>
       <c r="F18" t="n">
-        <v>1.7015621600056</v>
+        <v>1.70037246091027</v>
       </c>
       <c r="G18" t="n">
         <v>26</v>
       </c>
       <c r="H18" t="n">
-        <v>1.42348210431368</v>
+        <v>1.4235949643851</v>
       </c>
     </row>
     <row r="19">
@@ -867,13 +867,13 @@
         <v>23.719512195122</v>
       </c>
       <c r="F19" t="n">
-        <v>1.61298663182518</v>
+        <v>1.60199758409185</v>
       </c>
       <c r="G19" t="n">
         <v>23.5</v>
       </c>
       <c r="H19" t="n">
-        <v>2.01718716138192</v>
+        <v>2.03003079410757</v>
       </c>
     </row>
     <row r="20">
@@ -893,13 +893,13 @@
         <v>26.5978260869565</v>
       </c>
       <c r="F20" t="n">
-        <v>1.49476448346593</v>
+        <v>1.47293442595309</v>
       </c>
       <c r="G20" t="n">
         <v>26.5</v>
       </c>
       <c r="H20" t="n">
-        <v>1.75850222635062</v>
+        <v>1.76977855002148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>